<commit_message>
Going through preliminary analysis.
</commit_message>
<xml_diff>
--- a/ALL_DATA/TIFF_sediment/sediment_prelim.xlsx
+++ b/ALL_DATA/TIFF_sediment/sediment_prelim.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiff/Desktop/R Studio/APECS-master-repos/ALL_DATA/TIFF_sediment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31251DE9-522D-2B41-A825-E48A82F12045}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48222A1E-46BD-FE43-89FB-B6987B040AB3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5560" yWindow="0" windowWidth="28040" windowHeight="15760" xr2:uid="{1BF9C8A5-DB8B-6D4E-B16F-068FDF711835}"/>
   </bookViews>
@@ -519,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDFD578C-79E5-514C-89B6-0DE671F6B1F9}">
   <dimension ref="A1:M241"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A179" workbookViewId="0">
+      <selection activeCell="D207" sqref="D207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3866,7 +3866,7 @@
         <v>43322</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F82" s="1">
         <v>1</v>
@@ -3903,7 +3903,7 @@
         <v>43322</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F83" s="1">
         <v>2</v>
@@ -3940,7 +3940,7 @@
         <v>43322</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F84" s="1">
         <v>3</v>
@@ -3977,7 +3977,7 @@
         <v>43322</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F85" s="1">
         <v>4</v>
@@ -4014,7 +4014,7 @@
         <v>43322</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F86" s="1">
         <v>5</v>
@@ -8746,7 +8746,7 @@
         <v>43322</v>
       </c>
       <c r="E202" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F202" s="1">
         <v>1</v>
@@ -8783,7 +8783,7 @@
         <v>43322</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F203" s="1">
         <v>2</v>
@@ -8820,7 +8820,7 @@
         <v>43322</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F204" s="1">
         <v>3</v>
@@ -8857,7 +8857,7 @@
         <v>43322</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F205" s="1">
         <v>4</v>
@@ -8894,7 +8894,7 @@
         <v>43322</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F206" s="1">
         <v>5</v>

</xml_diff>